<commit_message>
excel updated  and  telangana name  removed
</commit_message>
<xml_diff>
--- a/public/employee_details.xlsx
+++ b/public/employee_details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manasa\Desktop\Fin7\dashboards_code\interim files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Aaro7\aaro7_ui\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BBA29E-DA2E-4850-9F14-CEE629CD0C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D16DAB-5301-4F7E-86B3-B90BA397F0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3710" windowWidth="19200" windowHeight="8620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Employee ID</t>
   </si>
@@ -55,10 +55,16 @@
     <t>Salary Type (Fixed/Variable)</t>
   </si>
   <si>
-    <t>Gross Salary</t>
-  </si>
-  <si>
-    <t>Net Salary</t>
+    <t>Net Salary (to be disbursed to the employee)</t>
+  </si>
+  <si>
+    <t>Employee Age</t>
+  </si>
+  <si>
+    <t>Gender(M/F)</t>
+  </si>
+  <si>
+    <t>CTC</t>
   </si>
 </sst>
 </file>
@@ -398,25 +404,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
-    <col min="2" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" customWidth="1"/>
-    <col min="12" max="12" width="27.26953125" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,40 +436,43 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>